<commit_message>
added files for 4/22
</commit_message>
<xml_diff>
--- a/Admin/Ara Folder/Spring Semester/Timesheet_3-6_3-12.xlsx
+++ b/Admin/Ara Folder/Spring Semester/Timesheet_3-6_3-12.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\borde\Senior Design Project\Admin\Ara Folder\Spring Semester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08FE4E69-A66C-4922-A31C-1AE30DF1B629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F82DCC47-D4B0-4B10-B6C7-7588E1FA739F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B1BC5497-AAD9-4DDC-8628-751A33E9D351}"/>
+    <workbookView xWindow="8400" yWindow="1248" windowWidth="17280" windowHeight="8964" xr2:uid="{B1BC5497-AAD9-4DDC-8628-751A33E9D351}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -546,8 +546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0F3F9F8-5E08-46D1-A043-3B52818921A7}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -717,13 +717,15 @@
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
+      <c r="E10" s="8">
+        <v>1</v>
+      </c>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
       <c r="H10" s="9"/>
       <c r="I10" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -767,13 +769,19 @@
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
+      <c r="E13" s="8">
+        <v>3</v>
+      </c>
       <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="9"/>
+      <c r="G13" s="8">
+        <v>2</v>
+      </c>
+      <c r="H13" s="9">
+        <v>1</v>
+      </c>
       <c r="I13" s="10">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -824,7 +832,7 @@
       </c>
       <c r="E16" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F16" s="10">
         <f t="shared" si="1"/>
@@ -832,15 +840,15 @@
       </c>
       <c r="G16" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H16" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I16" s="10">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">

</xml_diff>